<commit_message>
Ergebnisse vom 2. Spieltag ergänzt
</commit_message>
<xml_diff>
--- a/wg_clash_ergebnisse.xlsx
+++ b/wg_clash_ergebnisse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a750d02d39ef92fa/Dokumente/Basteleien/clash/clash_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{63415C27-B57A-4285-92C9-4583B82F4580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{077737FF-65EE-454B-AB3A-3AE9A95E686C}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{63415C27-B57A-4285-92C9-4583B82F4580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{748D499D-B1D6-440E-9E49-0053C568EAD0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{FCF13440-2A8C-4F0F-B769-A09D3F5D4E6A}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,6 +658,24 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="1">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -668,6 +686,18 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Ergebnisse 2. Spieltag korrigiert
</commit_message>
<xml_diff>
--- a/wg_clash_ergebnisse.xlsx
+++ b/wg_clash_ergebnisse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a750d02d39ef92fa/Dokumente/Basteleien/clash/clash_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{63415C27-B57A-4285-92C9-4583B82F4580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{748D499D-B1D6-440E-9E49-0053C568EAD0}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{63415C27-B57A-4285-92C9-4583B82F4580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62A25E92-54CF-4B9D-A62B-C368B576C9C3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{FCF13440-2A8C-4F0F-B769-A09D3F5D4E6A}"/>
   </bookViews>
@@ -668,10 +668,10 @@
         <v>18</v>
       </c>
       <c r="G6" s="1">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H6" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>

</xml_diff>